<commit_message>
Update + Timings spreadsheet
</commit_message>
<xml_diff>
--- a/BillofMaterials .xlsx
+++ b/BillofMaterials .xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="141">
   <si>
     <t>Liquid Handler</t>
   </si>
@@ -439,6 +439,9 @@
   </si>
   <si>
     <t>Tip Box for Tip Waste</t>
+  </si>
+  <si>
+    <t>http://nz.rs-online.com/web/p/fixed-height-mounts-feet/1034225/</t>
   </si>
 </sst>
 </file>
@@ -812,10 +815,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D154"/>
+  <dimension ref="B1:F154"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="G154" sqref="G154"/>
+      <selection activeCell="F154" sqref="F154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2159,7 +2162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
         <v>92</v>
       </c>
@@ -2170,7 +2173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
         <v>93</v>
       </c>
@@ -2181,7 +2184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B147" t="s">
         <v>94</v>
       </c>
@@ -2192,7 +2195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
         <v>95</v>
       </c>
@@ -2203,7 +2206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
         <v>78</v>
       </c>
@@ -2214,7 +2217,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="150" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
         <v>96</v>
       </c>
@@ -2222,7 +2225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
         <v>127</v>
       </c>
@@ -2233,7 +2236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
         <v>139</v>
       </c>
@@ -2241,7 +2244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
         <v>138</v>
       </c>
@@ -2250,6 +2253,9 @@
       </c>
       <c r="D154">
         <v>4</v>
+      </c>
+      <c r="F154" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>